<commit_message>
Atualização no script do liquibase
</commit_message>
<xml_diff>
--- a/src/test/resources/com/fatec/mom/test/documents/Codelist.xlsx
+++ b/src/test/resources/com/fatec/mom/test/documents/Codelist.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\facul\PI III\API\API_3sem_2021-01\src\test\resources\com\fatec\mom\test\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\facul\PI_III\API\API_3sem_2021-01\src\test\resources\com\fatec\mom\test\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="345" yWindow="540" windowWidth="20490" windowHeight="11385"/>
   </bookViews>
   <sheets>
-    <sheet name="ABC-1234" sheetId="1" r:id="rId1"/>
+    <sheet name="Teste-1234" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ABC-1234'!$A$1:$I$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Teste-1234'!$A$1:$I$27</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -913,7 +913,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>